<commit_message>
Updated the values after cross check
</commit_message>
<xml_diff>
--- a/Trace Link Quality SYSRS-SWRS/Case_Study_1_Evaluation_Pooling.xlsx
+++ b/Trace Link Quality SYSRS-SWRS/Case_Study_1_Evaluation_Pooling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvhi\Desktop\MasterThesis\chatgpt\Survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA7D368-575D-4467-A34E-9062AFBB6A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535DEEB8-FBE2-48A7-9E7C-9D5E31906764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B68AD377-0DE4-4BD0-894B-2E210DB609B6}"/>
   </bookViews>
@@ -2856,11 +2856,6 @@
 </t>
   </si>
   <si>
-    <t>1. Lack of detail on setting the status value.
-2. Lack of sequencing related to CRM_RCC and CRM_FCC.
-3. Source of status value parameter should be known.</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. no information on what happens when buffer is full i.e forget part.
 2. Not clear which data should be discarded new or old
 3, what to do if buffers are full is not present
@@ -2900,9 +2895,6 @@
 3.  This condition (waiting for CRM_CMD 0xA) is not present in SYSRS 010 or SYSRS 011 and adds complexity that the system requirements do not mention. </t>
   </si>
   <si>
-    <t>1. Default Value missing</t>
-  </si>
-  <si>
     <t>1. The software requirement should clarify whether comparing the RAM and NVM values of DSI3_physicalAddress is explicitly necessary based on system-level requirements.
 2. The introduction of the else condition (setting the error flag to 0x0) is additional and not required by the system requirement. This could be seen as an enhancement, but it does add functionality not explicitly covered in SYSRS 012.</t>
   </si>
@@ -3132,6 +3124,15 @@
 2. Inconsistency Between System and Software
 3. what is definition of valid?
 4. increment part Is not visible in sysrs</t>
+  </si>
+  <si>
+    <t>1. Default Value missing
+2. additional condition present which is not defined in sysrs</t>
+  </si>
+  <si>
+    <t>1. Lack of detail on setting the status value.
+2. Lack of sequencing related to CRM_RCC and CRM_FCC.
+3. Identify the Source of the Status Value</t>
   </si>
 </sst>
 </file>
@@ -3231,7 +3232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3295,6 +3296,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3407,7 +3414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3541,6 +3548,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5229,9 +5238,9 @@
   <dimension ref="A1:AH44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="R4" sqref="R4"/>
+      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="125.15" customHeight="1"/>
@@ -5611,19 +5620,19 @@
         <v>266</v>
       </c>
       <c r="R4" s="23" t="s">
-        <v>267</v>
+        <v>295</v>
       </c>
       <c r="S4">
         <v>2</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4">
         <v>0</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" s="22">
         <f t="shared" si="0"/>
@@ -5631,7 +5640,7 @@
       </c>
       <c r="X4" s="22">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AA4" t="s">
         <v>181</v>
@@ -5706,7 +5715,7 @@
         <v>233</v>
       </c>
       <c r="R5" s="23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -5798,10 +5807,10 @@
         <v>144</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="R6" s="23" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="S6">
         <v>2</v>
@@ -5813,7 +5822,7 @@
         <v>0</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6" s="22">
         <f t="shared" si="0"/>
@@ -5898,7 +5907,7 @@
         <v>234</v>
       </c>
       <c r="R7" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="S7">
         <v>1</v>
@@ -5991,7 +6000,7 @@
         <v>235</v>
       </c>
       <c r="R8" s="23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="S8">
         <v>0</v>
@@ -6000,7 +6009,7 @@
         <v>1</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -6085,10 +6094,10 @@
         <v>150</v>
       </c>
       <c r="Q9" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="R9" s="23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="S9">
         <v>3</v>
@@ -6180,7 +6189,7 @@
         <v>152</v>
       </c>
       <c r="Q10" s="26" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="R10" s="23" t="s">
         <v>173</v>
@@ -6282,7 +6291,7 @@
         <v>237</v>
       </c>
       <c r="R11" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S11">
         <v>3</v>
@@ -6305,7 +6314,7 @@
         <v>1</v>
       </c>
       <c r="AA11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="AB11">
         <v>0</v>
@@ -6372,16 +6381,16 @@
         <v>130</v>
       </c>
       <c r="Q12" s="26" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
       <c r="R12" s="23" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U12">
         <v>1</v>
@@ -6391,11 +6400,11 @@
       </c>
       <c r="W12" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X12" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AA12" t="s">
         <v>182</v>
@@ -6467,10 +6476,10 @@
         <v>132</v>
       </c>
       <c r="Q13" s="26" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="R13" s="23" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="S13">
         <v>1</v>
@@ -6482,7 +6491,7 @@
         <v>0</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13" s="22">
         <f t="shared" si="0"/>
@@ -6493,7 +6502,7 @@
         <v>1</v>
       </c>
       <c r="AA13" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AB13">
         <v>0</v>
@@ -6564,10 +6573,10 @@
         <v>134</v>
       </c>
       <c r="Q14" s="26" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="R14" s="23" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="S14">
         <v>1</v>
@@ -6661,10 +6670,10 @@
         <v>136</v>
       </c>
       <c r="Q15" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="R15" s="23" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="S15">
         <v>1</v>
@@ -6760,10 +6769,10 @@
         <v>126</v>
       </c>
       <c r="Q16" s="26" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="R16" s="23" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="S16">
         <v>1</v>
@@ -6859,10 +6868,10 @@
         <v>154</v>
       </c>
       <c r="Q17" s="26" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="R17" s="23" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="S17">
         <v>1</v>
@@ -6961,7 +6970,7 @@
         <v>259</v>
       </c>
       <c r="R18" s="23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="S18">
         <v>1</v>
@@ -7049,10 +7058,10 @@
         <v>158</v>
       </c>
       <c r="Q19" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="R19" s="23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="S19">
         <v>1</v>
@@ -7149,7 +7158,7 @@
         <v>175</v>
       </c>
       <c r="R20" s="23" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="S20">
         <v>1</v>
@@ -7197,7 +7206,7 @@
     </row>
     <row r="21" spans="1:33" ht="364.5" customHeight="1">
       <c r="A21" s="28" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B21" s="28" t="s">
         <v>46</v>
@@ -7244,7 +7253,7 @@
         <v>176</v>
       </c>
       <c r="R21" s="23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="S21">
         <v>2</v>
@@ -7298,36 +7307,36 @@
       <c r="L22"/>
       <c r="M22"/>
       <c r="N22"/>
-      <c r="S22">
+      <c r="S22" s="49">
         <f>SUM(S2:S21)</f>
-        <v>26</v>
-      </c>
-      <c r="T22">
+        <v>27</v>
+      </c>
+      <c r="T22" s="49">
         <f>SUM(T2:T21)</f>
         <v>11</v>
       </c>
-      <c r="U22">
+      <c r="U22" s="49">
         <f>SUM(U2:U21)</f>
-        <v>2</v>
-      </c>
-      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="V22" s="49">
         <f>SUM(V2:V21)</f>
-        <v>2</v>
-      </c>
-      <c r="W22" s="22">
+        <v>5</v>
+      </c>
+      <c r="W22" s="50">
         <f t="shared" si="0"/>
-        <v>0.9285714285714286</v>
-      </c>
-      <c r="X22" s="22">
+        <v>0.9642857142857143</v>
+      </c>
+      <c r="X22" s="50">
         <f t="shared" si="1"/>
-        <v>0.70270270270270274</v>
-      </c>
-      <c r="Y22" s="22">
+        <v>0.71052631578947367</v>
+      </c>
+      <c r="Y22" s="50">
         <f>(2*W22*X22)/(W22+X22)</f>
-        <v>0.79999999999999993</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="Z22" s="23" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AA22" s="23" t="s">
         <v>177</v>

</xml_diff>

<commit_message>
Deleted Sheet2 as it was not needed
</commit_message>
<xml_diff>
--- a/Trace Link Quality SYSRS-SWRS/Case_Study_1_Evaluation_Pooling.xlsx
+++ b/Trace Link Quality SYSRS-SWRS/Case_Study_1_Evaluation_Pooling.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvhi\Desktop\MasterThesis\chatgpt\Survey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvhi\Desktop\MasterThesis\FeasibilityStudyonChatGPTforRE\Trace Link Quality SYSRS-SWRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535DEEB8-FBE2-48A7-9E7C-9D5E31906764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC063E09-8EA4-428C-8BF4-49240F313EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B68AD377-0DE4-4BD0-894B-2E210DB609B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="296">
   <si>
     <t>System Requirement</t>
   </si>
@@ -3622,1302 +3621,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Recall</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="38100" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-6B52-4145-A733-4C64E86600AA}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-6B52-4145-A733-4C64E86600AA}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000004-6B52-4145-A733-4C64E86600AA}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="19"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-6B52-4145-A733-4C64E86600AA}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="20"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="00B050"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-6B52-4145-A733-4C64E86600AA}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-6B52-4145-A733-4C64E86600AA}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet2!$A$2:$A$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>7.9679999999999994E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2.101E-3</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-9.8480000000000009E-3</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.7429999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9.2700000000000005E-3</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="0.00">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20" formatCode="0.00">
-                  <c:v>0.86956521739130432</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet2!$B$2:$B$22</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.33333333333333331</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.66666666666666663</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.52631578947368418</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6B52-4145-A733-4C64E86600AA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1381497536"/>
-        <c:axId val="1381502816"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1381497536"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Precision</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1381502816"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1381502816"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Recall</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1381497536"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>92075</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>396875</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6053045C-2254-CD72-17A9-2814240953A9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5237,10 +3940,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54CDCBA-5A50-4075-92FE-949E47946B99}">
   <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="125.15" customHeight="1"/>
@@ -7500,199 +6203,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09D70F0A-069B-4C4F-A36C-81BAEBDF4381}">
-  <dimension ref="A1:B22"/>
-  <sheetViews>
-    <sheetView topLeftCell="C9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="2" width="12.453125" style="22" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>7.9679999999999994E-3</v>
-      </c>
-      <c r="B2" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>-2.101E-3</v>
-      </c>
-      <c r="B3" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="22">
-        <v>1</v>
-      </c>
-      <c r="B4" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="22">
-        <v>1</v>
-      </c>
-      <c r="B5" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="22">
-        <v>1</v>
-      </c>
-      <c r="B6" s="22">
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="22">
-        <v>1</v>
-      </c>
-      <c r="B7" s="22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>-9.8480000000000009E-3</v>
-      </c>
-      <c r="B8" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="22">
-        <v>1</v>
-      </c>
-      <c r="B9" s="22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="22">
-        <v>1</v>
-      </c>
-      <c r="B10" s="22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="22">
-        <v>1</v>
-      </c>
-      <c r="B11" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>7.7429999999999999E-3</v>
-      </c>
-      <c r="B12" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="22">
-        <v>1</v>
-      </c>
-      <c r="B13" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>9.2700000000000005E-3</v>
-      </c>
-      <c r="B14" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="22">
-        <v>1</v>
-      </c>
-      <c r="B15" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="22">
-        <v>1</v>
-      </c>
-      <c r="B16" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="22">
-        <v>1</v>
-      </c>
-      <c r="B17" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="22">
-        <v>1</v>
-      </c>
-      <c r="B18" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="22">
-        <v>1</v>
-      </c>
-      <c r="B19" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="22">
-        <v>1</v>
-      </c>
-      <c r="B20" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="22">
-        <v>1</v>
-      </c>
-      <c r="B21" s="22">
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="22">
-        <v>0.86956521739130432</v>
-      </c>
-      <c r="B22" s="22">
-        <v>0.52631578947368418</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added comment for minor finding
</commit_message>
<xml_diff>
--- a/Trace Link Quality SYSRS-SWRS/Case_Study_1_Evaluation_Pooling.xlsx
+++ b/Trace Link Quality SYSRS-SWRS/Case_Study_1_Evaluation_Pooling.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvhi\Desktop\MasterThesis\CaseStudyonChatGPTforRE\Trace Link Quality SYSRS-SWRS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vvhi\Desktop\Vibhashree_Master_Thesis\CaseStudyonChatGPTforRE\Trace Link Quality SYSRS-SWRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CD9BAC-5EE7-493E-BD13-FA8171BE5C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839B9800-638F-4C5C-82F1-6FD37C89174F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B68AD377-0DE4-4BD0-894B-2E210DB609B6}"/>
   </bookViews>
@@ -2828,12 +2828,6 @@
     </r>
   </si>
   <si>
-    <t>1. Connection between setting the register BRG.FS.f_s and actually digitizing could me explicity mentioned .
-2. Source of parameters missing.
-3. CRM_CMD condition not present in sysrs.
-4. What is Plus factor?</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. along with register setting, digitization should be ensured 
 </t>
   </si>
@@ -3132,6 +3126,12 @@
     <t>1. Lack of detail on setting the status value.
 2. Lack of sequencing related to CRM_RCC and CRM_FCC.
 3. Identify the Source of the Status Value</t>
+  </si>
+  <si>
+    <t>1. Connection between setting the register BRG.FS.f_s and actually digitizing could me explicity mentioned .
+2. Source of parameters missing.
+3. CRM_CMD condition not present in sysrs.
+4. What is Plus factor? (this finding ommitted because it was minor)</t>
   </si>
 </sst>
 </file>
@@ -3940,10 +3940,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54CDCBA-5A50-4075-92FE-949E47946B99}">
   <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="125.15" customHeight="1"/>
@@ -4121,10 +4121,10 @@
         <v>138</v>
       </c>
       <c r="Q2" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="R2" s="23" t="s">
         <v>262</v>
-      </c>
-      <c r="R2" s="23" t="s">
-        <v>263</v>
       </c>
       <c r="S2">
         <v>1</v>
@@ -4218,10 +4218,10 @@
         <v>140</v>
       </c>
       <c r="Q3" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="R3" s="23" t="s">
         <v>264</v>
-      </c>
-      <c r="R3" s="23" t="s">
-        <v>265</v>
       </c>
       <c r="S3">
         <v>2</v>
@@ -4320,10 +4320,10 @@
         <v>261</v>
       </c>
       <c r="Q4" s="26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="R4" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="S4">
         <v>2</v>
@@ -4418,7 +4418,7 @@
         <v>233</v>
       </c>
       <c r="R5" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -4510,10 +4510,10 @@
         <v>144</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="R6" s="23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="S6">
         <v>2</v>
@@ -4610,7 +4610,7 @@
         <v>234</v>
       </c>
       <c r="R7" s="23" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="S7">
         <v>1</v>
@@ -4703,7 +4703,7 @@
         <v>235</v>
       </c>
       <c r="R8" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="S8">
         <v>0</v>
@@ -4797,10 +4797,10 @@
         <v>150</v>
       </c>
       <c r="Q9" s="26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="R9" s="23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="S9">
         <v>3</v>
@@ -4892,7 +4892,7 @@
         <v>152</v>
       </c>
       <c r="Q10" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="R10" s="23" t="s">
         <v>173</v>
@@ -4994,7 +4994,7 @@
         <v>237</v>
       </c>
       <c r="R11" s="26" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="S11">
         <v>3</v>
@@ -5017,7 +5017,7 @@
         <v>1</v>
       </c>
       <c r="AA11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AB11">
         <v>0</v>
@@ -5084,10 +5084,10 @@
         <v>130</v>
       </c>
       <c r="Q12" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="R12" s="23" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S12">
         <v>1</v>
@@ -5179,10 +5179,10 @@
         <v>132</v>
       </c>
       <c r="Q13" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="R13" s="23" t="s">
         <v>277</v>
-      </c>
-      <c r="R13" s="23" t="s">
-        <v>278</v>
       </c>
       <c r="S13">
         <v>1</v>
@@ -5205,7 +5205,7 @@
         <v>1</v>
       </c>
       <c r="AA13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AB13">
         <v>0</v>
@@ -5276,10 +5276,10 @@
         <v>134</v>
       </c>
       <c r="Q14" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R14" s="23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="S14">
         <v>1</v>
@@ -5373,10 +5373,10 @@
         <v>136</v>
       </c>
       <c r="Q15" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="R15" s="23" t="s">
         <v>279</v>
-      </c>
-      <c r="R15" s="23" t="s">
-        <v>280</v>
       </c>
       <c r="S15">
         <v>1</v>
@@ -5472,10 +5472,10 @@
         <v>126</v>
       </c>
       <c r="Q16" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="R16" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S16">
         <v>1</v>
@@ -5571,10 +5571,10 @@
         <v>154</v>
       </c>
       <c r="Q17" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="R17" s="23" t="s">
         <v>281</v>
-      </c>
-      <c r="R17" s="23" t="s">
-        <v>282</v>
       </c>
       <c r="S17">
         <v>1</v>
@@ -5673,7 +5673,7 @@
         <v>259</v>
       </c>
       <c r="R18" s="23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="S18">
         <v>1</v>
@@ -5761,10 +5761,10 @@
         <v>158</v>
       </c>
       <c r="Q19" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="R19" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="S19">
         <v>1</v>
@@ -5861,7 +5861,7 @@
         <v>175</v>
       </c>
       <c r="R20" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="S20">
         <v>1</v>
@@ -5909,7 +5909,7 @@
     </row>
     <row r="21" spans="1:33" ht="364.5" customHeight="1">
       <c r="A21" s="28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B21" s="28" t="s">
         <v>46</v>
@@ -5956,7 +5956,7 @@
         <v>176</v>
       </c>
       <c r="R21" s="23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="S21">
         <v>2</v>
@@ -6039,7 +6039,7 @@
         <v>0.81818181818181823</v>
       </c>
       <c r="Z22" s="23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AA22" s="23" t="s">
         <v>177</v>

</xml_diff>